<commit_message>
yprime created and excel file updated
</commit_message>
<xml_diff>
--- a/files/exp.xlsx
+++ b/files/exp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Education and Skills\KNTU science community\Super Course AI\Chapter 1\Homework\Ch01_HW01\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FDF1246-59D3-4F5B-AE5F-C27FBA221CF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE6F4D0-7C44-4F49-8560-EE908E1E08FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -340,608 +340,492 @@
   <dimension ref="A1:B60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18.796875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
       <c r="B1">
-        <f>EXP(A1)</f>
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <f>A1+0.1</f>
         <v>0.1</v>
       </c>
       <c r="B2">
-        <f t="shared" ref="B2:B60" si="0">EXP(A2)</f>
-        <v>1.1051709180756477</v>
+        <v>1.105</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f t="shared" ref="A3:A60" si="1">A2+0.1</f>
         <v>0.2</v>
       </c>
       <c r="B3">
-        <f t="shared" si="0"/>
-        <v>1.2214027581601699</v>
+        <v>1.2210000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" si="1"/>
-        <v>0.30000000000000004</v>
+        <v>0.3</v>
       </c>
       <c r="B4">
-        <f t="shared" si="0"/>
-        <v>1.3498588075760032</v>
+        <v>1.35</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
       <c r="B5">
-        <f t="shared" si="0"/>
-        <v>1.4918246976412703</v>
+        <v>1.492</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="B6">
-        <f t="shared" si="0"/>
-        <v>1.6487212707001282</v>
+        <v>1.649</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
       <c r="B7">
-        <f t="shared" si="0"/>
-        <v>1.8221188003905089</v>
+        <v>1.8220000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f t="shared" si="1"/>
         <v>0.7</v>
       </c>
       <c r="B8">
-        <f t="shared" si="0"/>
-        <v>2.0137527074704766</v>
+        <v>2.0139999999999998</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f t="shared" si="1"/>
-        <v>0.79999999999999993</v>
+        <v>0.8</v>
       </c>
       <c r="B9">
-        <f t="shared" si="0"/>
-        <v>2.2255409284924674</v>
+        <v>2.226</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f t="shared" si="1"/>
-        <v>0.89999999999999991</v>
+        <v>0.9</v>
       </c>
       <c r="B10">
-        <f t="shared" si="0"/>
-        <v>2.4596031111569494</v>
+        <v>2.46</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f t="shared" si="1"/>
-        <v>0.99999999999999989</v>
+        <v>1</v>
       </c>
       <c r="B11">
-        <f t="shared" si="0"/>
-        <v>2.7182818284590451</v>
+        <v>2.718</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f t="shared" si="1"/>
-        <v>1.0999999999999999</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="B12">
-        <f t="shared" si="0"/>
-        <v>3.0041660239464325</v>
+        <v>3.004</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f t="shared" si="1"/>
         <v>1.2</v>
       </c>
       <c r="B13">
-        <f t="shared" si="0"/>
-        <v>3.3201169227365472</v>
+        <v>3.32</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f t="shared" si="1"/>
         <v>1.3</v>
       </c>
       <c r="B14">
-        <f t="shared" si="0"/>
-        <v>3.6692966676192444</v>
+        <v>3.67</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f t="shared" si="1"/>
-        <v>1.4000000000000001</v>
+        <v>1.4</v>
       </c>
       <c r="B15">
-        <f t="shared" si="0"/>
-        <v>4.0551999668446754</v>
+        <v>4.0549999999999997</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f t="shared" si="1"/>
-        <v>1.5000000000000002</v>
+        <v>1.5</v>
       </c>
       <c r="B16">
-        <f t="shared" si="0"/>
-        <v>4.4816890703380654</v>
+        <v>4.4820000000000002</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f t="shared" si="1"/>
-        <v>1.6000000000000003</v>
+        <v>1.6</v>
       </c>
       <c r="B17">
-        <f t="shared" si="0"/>
-        <v>4.9530324243951167</v>
+        <v>4.9530000000000003</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f t="shared" si="1"/>
-        <v>1.7000000000000004</v>
+        <v>1.7</v>
       </c>
       <c r="B18">
-        <f t="shared" si="0"/>
-        <v>5.4739473917272017</v>
+        <v>5.4740000000000002</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f t="shared" si="1"/>
-        <v>1.8000000000000005</v>
+        <v>1.8</v>
       </c>
       <c r="B19">
-        <f t="shared" si="0"/>
-        <v>6.0496474644129492</v>
+        <v>6.05</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f t="shared" si="1"/>
-        <v>1.9000000000000006</v>
+        <v>1.9</v>
       </c>
       <c r="B20">
-        <f t="shared" si="0"/>
-        <v>6.685894442279273</v>
+        <v>6.6859999999999999</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f t="shared" si="1"/>
-        <v>2.0000000000000004</v>
+        <v>2</v>
       </c>
       <c r="B21">
-        <f t="shared" si="0"/>
-        <v>7.3890560989306531</v>
+        <v>7.3890000000000002</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f t="shared" si="1"/>
-        <v>2.1000000000000005</v>
+        <v>2.1</v>
       </c>
       <c r="B22">
-        <f t="shared" si="0"/>
-        <v>8.1661699125676552</v>
+        <v>8.1660000000000004</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f t="shared" si="1"/>
-        <v>2.2000000000000006</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="B23">
-        <f t="shared" si="0"/>
-        <v>9.0250134994341273</v>
+        <v>9.0250000000000004</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f t="shared" si="1"/>
-        <v>2.3000000000000007</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="B24">
-        <f t="shared" si="0"/>
-        <v>9.9741824548147271</v>
+        <v>9.9740000000000002</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f t="shared" si="1"/>
-        <v>2.4000000000000008</v>
+        <v>2.4</v>
       </c>
       <c r="B25">
-        <f t="shared" si="0"/>
-        <v>11.02317638064161</v>
+        <v>11.023</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f t="shared" si="1"/>
-        <v>2.5000000000000009</v>
+        <v>2.5</v>
       </c>
       <c r="B26">
-        <f t="shared" si="0"/>
-        <v>12.182493960703484</v>
+        <v>12.182</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f t="shared" si="1"/>
-        <v>2.600000000000001</v>
+        <v>2.6</v>
       </c>
       <c r="B27">
-        <f t="shared" si="0"/>
-        <v>13.463738035001704</v>
+        <v>13.464</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f t="shared" si="1"/>
-        <v>2.7000000000000011</v>
+        <v>2.7</v>
       </c>
       <c r="B28">
-        <f t="shared" si="0"/>
-        <v>14.879731724872849</v>
+        <v>14.88</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
-        <f t="shared" si="1"/>
-        <v>2.8000000000000012</v>
+        <v>2.8</v>
       </c>
       <c r="B29">
-        <f t="shared" si="0"/>
-        <v>16.444646771097069</v>
+        <v>16.445</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f t="shared" si="1"/>
-        <v>2.9000000000000012</v>
+        <v>2.9</v>
       </c>
       <c r="B30">
-        <f t="shared" si="0"/>
-        <v>18.174145369443085</v>
+        <v>18.173999999999999</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
-        <f t="shared" si="1"/>
-        <v>3.0000000000000013</v>
+        <v>3</v>
       </c>
       <c r="B31">
-        <f t="shared" si="0"/>
-        <v>20.085536923187693</v>
+        <v>20.085999999999999</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
-        <f t="shared" si="1"/>
-        <v>3.1000000000000014</v>
+        <v>3.1</v>
       </c>
       <c r="B32">
-        <f t="shared" si="0"/>
-        <v>22.197951281441664</v>
+        <v>22.198</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f t="shared" si="1"/>
-        <v>3.2000000000000015</v>
+        <v>3.2</v>
       </c>
       <c r="B33">
-        <f t="shared" si="0"/>
-        <v>24.532530197109384</v>
+        <v>24.533000000000001</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
-        <f t="shared" si="1"/>
-        <v>3.3000000000000016</v>
+        <v>3.3</v>
       </c>
       <c r="B34">
-        <f t="shared" si="0"/>
-        <v>27.112638920657929</v>
+        <v>27.111999999999998</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
-        <f t="shared" si="1"/>
-        <v>3.4000000000000017</v>
+        <v>3.4</v>
       </c>
       <c r="B35">
-        <f t="shared" si="0"/>
-        <v>29.964100047397064</v>
+        <v>29.963999999999999</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
-        <f t="shared" si="1"/>
-        <v>3.5000000000000018</v>
+        <v>3.5</v>
       </c>
       <c r="B36">
-        <f t="shared" si="0"/>
-        <v>33.115451958692375</v>
+        <v>33.115000000000002</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
-        <f t="shared" si="1"/>
-        <v>3.6000000000000019</v>
+        <v>3.6</v>
       </c>
       <c r="B37">
-        <f t="shared" si="0"/>
-        <v>36.598234443678059</v>
+        <v>36.597999999999999</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
-        <f t="shared" si="1"/>
-        <v>3.700000000000002</v>
+        <v>3.7</v>
       </c>
       <c r="B38">
-        <f t="shared" si="0"/>
-        <v>40.44730436006747</v>
+        <v>40.447000000000003</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
-        <f t="shared" si="1"/>
-        <v>3.800000000000002</v>
+        <v>3.8</v>
       </c>
       <c r="B39">
-        <f t="shared" si="0"/>
-        <v>44.701184493300914</v>
+        <v>44.701000000000001</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
-        <f t="shared" si="1"/>
-        <v>3.9000000000000021</v>
+        <v>3.9</v>
       </c>
       <c r="B40">
-        <f t="shared" si="0"/>
-        <v>49.40244910553028</v>
+        <v>49.402000000000001</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
-        <f t="shared" si="1"/>
-        <v>4.0000000000000018</v>
+        <v>4</v>
       </c>
       <c r="B41">
-        <f t="shared" si="0"/>
-        <v>54.598150033144336</v>
+        <v>54.597999999999999</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
-        <f t="shared" si="1"/>
-        <v>4.1000000000000014</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="B42">
-        <f t="shared" si="0"/>
-        <v>60.340287597362057</v>
+        <v>60.34</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
-        <f t="shared" si="1"/>
-        <v>4.2000000000000011</v>
+        <v>4.2</v>
       </c>
       <c r="B43">
-        <f t="shared" si="0"/>
-        <v>66.686331040925211</v>
+        <v>66.686000000000007</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
-        <f t="shared" si="1"/>
-        <v>4.3000000000000007</v>
+        <v>4.3</v>
       </c>
       <c r="B44">
-        <f t="shared" si="0"/>
-        <v>73.699793699595844</v>
+        <v>73.7</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
-        <f t="shared" si="1"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="B45">
-        <f t="shared" si="0"/>
-        <v>81.450868664968141</v>
+        <v>81.450999999999993</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
-        <f t="shared" si="1"/>
         <v>4.5</v>
       </c>
       <c r="B46">
-        <f t="shared" si="0"/>
-        <v>90.017131300521811</v>
+        <v>90.016999999999996</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
-        <f t="shared" si="1"/>
         <v>4.5999999999999996</v>
       </c>
       <c r="B47">
-        <f t="shared" si="0"/>
-        <v>99.484315641933776</v>
+        <v>99.483999999999995</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
-        <f t="shared" si="1"/>
-        <v>4.6999999999999993</v>
+        <v>4.7</v>
       </c>
       <c r="B48">
-        <f t="shared" si="0"/>
-        <v>109.94717245212343</v>
+        <v>109.947</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
-        <f t="shared" si="1"/>
-        <v>4.7999999999999989</v>
+        <v>4.8</v>
       </c>
       <c r="B49">
-        <f t="shared" si="0"/>
-        <v>121.51041751873476</v>
+        <v>121.51</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
-        <f t="shared" si="1"/>
-        <v>4.8999999999999986</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="B50">
-        <f t="shared" si="0"/>
-        <v>134.2897796849353</v>
+        <v>134.29</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
-        <f t="shared" si="1"/>
-        <v>4.9999999999999982</v>
+        <v>5</v>
       </c>
       <c r="B51">
-        <f t="shared" si="0"/>
-        <v>148.41315910257634</v>
+        <v>148.41300000000001</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
-        <f t="shared" si="1"/>
-        <v>5.0999999999999979</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="B52">
-        <f t="shared" si="0"/>
-        <v>164.02190729990139</v>
+        <v>164.02199999999999</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53">
-        <f t="shared" si="1"/>
-        <v>5.1999999999999975</v>
+        <v>5.2</v>
       </c>
       <c r="B53">
-        <f t="shared" si="0"/>
-        <v>181.27224187515074</v>
+        <v>181.27199999999999</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54">
-        <f t="shared" si="1"/>
-        <v>5.2999999999999972</v>
+        <v>5.3</v>
       </c>
       <c r="B54">
-        <f t="shared" si="0"/>
-        <v>200.33680997479112</v>
+        <v>200.33699999999999</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
-        <f t="shared" si="1"/>
-        <v>5.3999999999999968</v>
+        <v>5.4</v>
       </c>
       <c r="B55">
-        <f t="shared" si="0"/>
-        <v>221.40641620418637</v>
+        <v>221.40700000000001</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56">
-        <f t="shared" si="1"/>
-        <v>5.4999999999999964</v>
+        <v>5.5</v>
       </c>
       <c r="B56">
-        <f t="shared" si="0"/>
-        <v>244.69193226421953</v>
+        <v>244.69200000000001</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
-        <f t="shared" si="1"/>
-        <v>5.5999999999999961</v>
+        <v>5.6</v>
       </c>
       <c r="B57">
-        <f t="shared" si="0"/>
-        <v>270.42640742615157</v>
+        <v>270.42599999999999</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58">
-        <f t="shared" si="1"/>
-        <v>5.6999999999999957</v>
+        <v>5.7</v>
       </c>
       <c r="B58">
-        <f t="shared" si="0"/>
-        <v>298.86740096705898</v>
+        <v>298.86700000000002</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59">
-        <f t="shared" si="1"/>
-        <v>5.7999999999999954</v>
+        <v>5.8</v>
       </c>
       <c r="B59">
-        <f t="shared" si="0"/>
-        <v>330.29955990964714</v>
+        <v>330.3</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60">
-        <f t="shared" si="1"/>
-        <v>5.899999999999995</v>
+        <v>5.9</v>
       </c>
       <c r="B60">
-        <f t="shared" si="0"/>
-        <v>365.03746786532696</v>
+        <v>365.03699999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>